<commit_message>
add es plots by moderator based on es diffs
</commit_message>
<xml_diff>
--- a/Effect size coding (online testing MA).xlsx
+++ b/Effect size coding (online testing MA).xlsx
@@ -8,11 +8,11 @@
     <sheet state="visible" name="Methods" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_DCDEDB20_DE13_4449_B7C3_C53D649046F6_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_F6ADD85A_D780_48A2_813B_F3CFEE6598D2_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DCDEDB20-DE13-4449-B7C3-C53D649046F6}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F6ADD85A-D780-48A2-813B-F3CFEE6598D2}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -17456,7 +17456,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DCDEDB20-DE13-4449-B7C3-C53D649046F6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F6ADD85A-D780-48A2-813B-F3CFEE6598D2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AJ$90"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Update Effect size coding (online testing MA).xlsx
</commit_message>
<xml_diff>
--- a/Effect size coding (online testing MA).xlsx
+++ b/Effect size coding (online testing MA).xlsx
@@ -10,12 +10,12 @@
     <sheet state="visible" name="Study-level comparison codebook" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_A629AC92_DDA3_493F_8955_BE0759204FA7_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
-    <definedName hidden="1" localSheetId="3" name="Z_A629AC92_DDA3_493F_8955_BE0759204FA7_.wvu.FilterData">'Study-level comparison coding'!$A$1:$I$10</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_682BB038_424F_4B43_B943_47FAC9632588_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
+    <definedName hidden="1" localSheetId="3" name="Z_682BB038_424F_4B43_B943_47FAC9632588_.wvu.FilterData">'Study-level comparison coding'!$A$1:$I$10</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A629AC92-DDA3-493F-8955-BE0759204FA7}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{682BB038-424F-4B43-B943-47FAC9632588}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -22635,7 +22635,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{A629AC92-DDA3-493F-8955-BE0759204FA7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{682BB038-424F-4B43-B943-47FAC9632588}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AJ$90"/>
     </customSheetView>
   </customSheetViews>
@@ -27718,7 +27718,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{A629AC92-DDA3-493F-8955-BE0759204FA7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{682BB038-424F-4B43-B943-47FAC9632588}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$10"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
updated nested random effects
</commit_message>
<xml_diff>
--- a/Effect size coding (online testing MA).xlsx
+++ b/Effect size coding (online testing MA).xlsx
@@ -10,12 +10,12 @@
     <sheet state="visible" name="Study-level comparison codebook" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_D530A1B4_C9F5_42F3_AD02_60CCF01937FA_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
-    <definedName hidden="1" localSheetId="3" name="Z_D530A1B4_C9F5_42F3_AD02_60CCF01937FA_.wvu.FilterData">'Study-level comparison coding'!$A$1:$I$10</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0CEF9939_AF13_4A58_9D86_715D7A35DB69_.wvu.FilterData">Data!$A$1:$AJ$90</definedName>
+    <definedName hidden="1" localSheetId="3" name="Z_0CEF9939_AF13_4A58_9D86_715D7A35DB69_.wvu.FilterData">'Study-level comparison coding'!$A$1:$I$10</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D530A1B4-C9F5-42F3-AD02-60CCF01937FA}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0CEF9939-AF13-4A58-9D86-715D7A35DB69}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3712" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3718" uniqueCount="670">
   <si>
     <t>paper_ID</t>
   </si>
@@ -879,12 +879,18 @@
     <t>Online measures of looking and learning in infancy</t>
   </si>
   <si>
+    <t>Observing the unexpected enhances infants’ learning and exploration</t>
+  </si>
+  <si>
     <t>AS Smith‐Flores, J Perez, MH Zhang, L Feigenson</t>
   </si>
   <si>
     <t>smith2022online</t>
   </si>
   <si>
+    <t>stahl2015observing</t>
+  </si>
+  <si>
     <t>https://alexisssmith.files.wordpress.com/2021/09/smithfloresperezzhangfeigenson2021.pdf</t>
   </si>
   <si>
@@ -898,12 +904,6 @@
   </si>
   <si>
     <t>expt 1b isn't direct replication, it's more building, but 1a is direct</t>
-  </si>
-  <si>
-    <t>Observing the unexpected enhances infants’ learning and exploration</t>
-  </si>
-  <si>
-    <t>stahl2015observing</t>
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5861377/</t>
@@ -4102,7 +4102,7 @@
         <v>14.0</v>
       </c>
       <c r="B18" s="7">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>88</v>
@@ -4183,7 +4183,7 @@
         <v>14.0</v>
       </c>
       <c r="B19" s="7">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>88</v>
@@ -9967,12 +9967,17 @@
       <c r="C89" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D89" s="17"/>
+      <c r="D89" s="32" t="s">
+        <v>182</v>
+      </c>
       <c r="E89" s="18" t="s">
         <v>172</v>
       </c>
       <c r="F89" s="9" t="s">
         <v>173</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H89" s="22" t="s">
         <v>180</v>
@@ -10046,12 +10051,17 @@
       <c r="C90" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="D90" s="17"/>
+      <c r="D90" s="32" t="s">
+        <v>182</v>
+      </c>
       <c r="E90" s="18" t="s">
         <v>172</v>
       </c>
       <c r="F90" s="9" t="s">
         <v>173</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="H90" s="22" t="s">
         <v>180</v>
@@ -11292,7 +11302,7 @@
         <v>202.0</v>
       </c>
       <c r="B104" s="25">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="C104" s="26" t="s">
         <v>261</v>
@@ -11384,7 +11394,7 @@
         <v>202.0</v>
       </c>
       <c r="B105" s="25">
-        <v>37.0</v>
+        <v>36.0</v>
       </c>
       <c r="C105" s="26" t="s">
         <v>261</v>
@@ -11481,26 +11491,32 @@
       <c r="C106" s="38" t="s">
         <v>273</v>
       </c>
+      <c r="D106" s="9" t="s">
+        <v>274</v>
+      </c>
       <c r="E106" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>277</v>
       </c>
       <c r="H106" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I106" s="9" t="s">
         <v>41</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L106" s="9" t="s">
         <v>42</v>
       </c>
       <c r="M106" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N106" s="9">
         <v>51.0</v>
@@ -11515,7 +11531,7 @@
         <v>46</v>
       </c>
       <c r="S106" s="9" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="T106" s="9" t="s">
         <v>84</v>
@@ -11546,7 +11562,7 @@
         <v>0.0642</v>
       </c>
       <c r="AJ106" s="9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AK106" s="30" t="s">
         <v>144</v>
@@ -11563,19 +11579,19 @@
         <v>273</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E107" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H107" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I107" s="9" t="s">
         <v>41</v>
@@ -11584,7 +11600,7 @@
         <v>283</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L107" s="9" t="s">
         <v>50</v>
@@ -11605,7 +11621,7 @@
         <v>46</v>
       </c>
       <c r="S107" s="9" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="T107" s="9" t="s">
         <v>84</v>
@@ -11662,19 +11678,19 @@
         <v>273</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E108" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H108" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I108" s="9" t="s">
         <v>41</v>
@@ -11686,7 +11702,7 @@
         <v>42</v>
       </c>
       <c r="M108" s="9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="N108" s="9">
         <v>52.0</v>
@@ -11746,19 +11762,19 @@
         <v>273</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E109" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H109" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I109" s="9" t="s">
         <v>41</v>
@@ -11845,19 +11861,19 @@
         <v>273</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="E110" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H110" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I110" s="9" t="s">
         <v>41</v>
@@ -13032,7 +13048,7 @@
         <v>279.0</v>
       </c>
       <c r="B125" s="41">
-        <v>45.0</v>
+        <v>46.0</v>
       </c>
       <c r="C125" s="38" t="s">
         <v>318</v>
@@ -13109,7 +13125,7 @@
         <v>279.0</v>
       </c>
       <c r="B126" s="41">
-        <v>45.0</v>
+        <v>46.0</v>
       </c>
       <c r="C126" s="38" t="s">
         <v>318</v>
@@ -13186,7 +13202,7 @@
         <v>279.0</v>
       </c>
       <c r="B127" s="41">
-        <v>45.0</v>
+        <v>47.0</v>
       </c>
       <c r="C127" s="38" t="s">
         <v>318</v>
@@ -13263,7 +13279,7 @@
         <v>279.0</v>
       </c>
       <c r="B128" s="41">
-        <v>45.0</v>
+        <v>47.0</v>
       </c>
       <c r="C128" s="38" t="s">
         <v>318</v>
@@ -13340,7 +13356,7 @@
         <v>279.0</v>
       </c>
       <c r="B129" s="41">
-        <v>45.0</v>
+        <v>48.0</v>
       </c>
       <c r="C129" s="38" t="s">
         <v>318</v>
@@ -13417,7 +13433,7 @@
         <v>279.0</v>
       </c>
       <c r="B130" s="41">
-        <v>45.0</v>
+        <v>48.0</v>
       </c>
       <c r="C130" s="38" t="s">
         <v>318</v>
@@ -13494,7 +13510,7 @@
         <v>279.0</v>
       </c>
       <c r="B131" s="41">
-        <v>45.0</v>
+        <v>49.0</v>
       </c>
       <c r="C131" s="38" t="s">
         <v>318</v>
@@ -13571,7 +13587,7 @@
         <v>279.0</v>
       </c>
       <c r="B132" s="41">
-        <v>45.0</v>
+        <v>49.0</v>
       </c>
       <c r="C132" s="38" t="s">
         <v>318</v>
@@ -13648,7 +13664,7 @@
         <v>315.0</v>
       </c>
       <c r="B133" s="9">
-        <v>47.0</v>
+        <v>61.0</v>
       </c>
       <c r="C133" s="38" t="s">
         <v>330</v>
@@ -13732,7 +13748,7 @@
         <v>315.0</v>
       </c>
       <c r="B134" s="9">
-        <v>47.0</v>
+        <v>61.0</v>
       </c>
       <c r="C134" s="38" t="s">
         <v>330</v>
@@ -13819,7 +13835,7 @@
         <v>315.0</v>
       </c>
       <c r="B135" s="9">
-        <v>47.0</v>
+        <v>61.0</v>
       </c>
       <c r="C135" s="38" t="s">
         <v>330</v>
@@ -13903,7 +13919,7 @@
         <v>317.0</v>
       </c>
       <c r="B136" s="41">
-        <v>48.0</v>
+        <v>62.0</v>
       </c>
       <c r="C136" s="38" t="s">
         <v>345</v>
@@ -13977,7 +13993,7 @@
         <v>317.0</v>
       </c>
       <c r="B137" s="41">
-        <v>48.0</v>
+        <v>62.0</v>
       </c>
       <c r="C137" s="38" t="s">
         <v>345</v>
@@ -20166,7 +20182,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D530A1B4-C9F5-42F3-AD02-60CCF01937FA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0CEF9939-AF13-4A58-9D86-715D7A35DB69}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$AJ$90"/>
     </customSheetView>
   </customSheetViews>
@@ -22155,13 +22171,13 @@
         <v>273</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G17" s="40"/>
       <c r="H17" s="34" t="s">
@@ -25250,7 +25266,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{D530A1B4-C9F5-42F3-AD02-60CCF01937FA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0CEF9939-AF13-4A58-9D86-715D7A35DB69}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$I$10"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>